<commit_message>
Activated PageProcessor. Added SCRIPT capabilities (column).
</commit_message>
<xml_diff>
--- a/documentation/Examples/WebNavigation/TestNavigations.xlsx
+++ b/documentation/Examples/WebNavigation/TestNavigations.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t xml:space="preserve">RUN</t>
   </si>
@@ -60,7 +60,10 @@
     <t xml:space="preserve">QA</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;@!!{xpath=//*[contains(text(),'Hello. Sign in')]}&gt;</t>
+    <t xml:space="preserve">SCRIPT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;@!{xpath=//*[contains(text(),'Hello. Sign in')]}&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">xpath=//h1[contains(text(),'Sign in')]</t>
@@ -69,34 +72,28 @@
     <t xml:space="preserve">Sign in</t>
   </si>
   <si>
-    <t xml:space="preserve">y</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">gpawel17@mail</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.com|1qazxsw2!</t>
-    </r>
+    <t xml:space="preserve">try { logs.info(“\n\n HI \n\n”);} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gpawel17@mail.com|1qazxsw2!</t>
   </si>
   <si>
     <t xml:space="preserve">xpath=//*[@id='nav-link-yourAccount']/span[1]</t>
   </si>
   <si>
     <t xml:space="preserve">Hello, Pavel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;@!{xpath=//*[@id='twotabsearchtextbox']}&gt;|hair {SPACE} brash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xpath=//*[@id=’didYouMean’]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Showing results for</t>
   </si>
 </sst>
 </file>
@@ -105,7 +102,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -179,12 +176,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -217,13 +218,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.6632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.2602040816326"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -284,7 +285,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -337,18 +340,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.7959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.64285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3724489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="31.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.9081632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -358,7 +362,7 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
@@ -368,6 +372,9 @@
         <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>5</v>
       </c>
     </row>
@@ -375,33 +382,50 @@
       <c r="A2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>12</v>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="D3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>18</v>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" display="gpawel17@mail"/>
+    <hyperlink ref="C3" r:id="rId1" display="gpawel17@mail.com|1qazxsw2!"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>